<commit_message>
adding tests to be better
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
+++ b/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\BIDS-converter\Metadata_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galassiae/Projects/PET2BIDS/spreadsheet_conversion/single_subject_sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6621B04B-DC62-40EA-AD7C-D00022C2DFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C779BE8-24A2-0444-870D-AC84706497AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -175,13 +180,25 @@
   </si>
   <si>
     <t>Neurobiology Research Unit</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>plasma_radioactivity</t>
+  </si>
+  <si>
+    <t>metabolite_parent_fraction</t>
+  </si>
+  <si>
+    <t>whole_blood_radioactivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,8 +206,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +224,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,11 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +267,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,13 +570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
-  <dimension ref="A1:AC46"/>
+  <dimension ref="A1:AG46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
@@ -569,9 +604,12 @@
     <col min="27" max="27" width="27.83203125" customWidth="1"/>
     <col min="28" max="28" width="15.6640625" customWidth="1"/>
     <col min="29" max="29" width="25.83203125" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,8 +697,20 @@
       <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -748,8 +798,20 @@
       <c r="AC2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD2" s="5">
+        <v>16.200000000000003</v>
+      </c>
+      <c r="AE2">
+        <v>32.35522376080818</v>
+      </c>
+      <c r="AF2">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG2">
+        <v>11.167945849940288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P3">
         <v>10</v>
       </c>
@@ -765,144 +827,360 @@
       <c r="X3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD3" s="5">
+        <v>28.2</v>
+      </c>
+      <c r="AE3">
+        <v>2507.1051839992842</v>
+      </c>
+      <c r="AF3">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG3">
+        <v>4027.7881549527583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P4">
         <v>20</v>
       </c>
       <c r="Q4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD4" s="5">
+        <v>42</v>
+      </c>
+      <c r="AE4">
+        <v>30219.040354280194</v>
+      </c>
+      <c r="AF4">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG4">
+        <v>36565.981242480346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P5">
         <v>30</v>
       </c>
       <c r="Q5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD5" s="5">
+        <v>58.8</v>
+      </c>
+      <c r="AE5">
+        <v>49458.133946955189</v>
+      </c>
+      <c r="AF5">
+        <v>0.987721971939862</v>
+      </c>
+      <c r="AG5">
+        <v>49458.133946955189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P6">
         <v>40</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD6" s="5">
+        <v>73.8</v>
+      </c>
+      <c r="AE6">
+        <v>54625.128373263819</v>
+      </c>
+      <c r="AF6">
+        <v>0.98277401617497218</v>
+      </c>
+      <c r="AG6">
+        <v>77625.006110518632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P7">
         <v>50</v>
       </c>
       <c r="Q7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD7" s="5">
+        <v>88.8</v>
+      </c>
+      <c r="AE7">
+        <v>59463.809533870204</v>
+      </c>
+      <c r="AF7">
+        <v>0.97465638230006379</v>
+      </c>
+      <c r="AG7">
+        <v>84130.176446829675</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P8">
         <v>60</v>
       </c>
       <c r="Q8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD8" s="5">
+        <v>105</v>
+      </c>
+      <c r="AE8">
+        <v>64473.636151116443</v>
+      </c>
+      <c r="AF8">
+        <v>0.97426988808824744</v>
+      </c>
+      <c r="AG8">
+        <v>88701.158697802806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P9">
         <v>80</v>
       </c>
       <c r="Q9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD9" s="5">
+        <v>118.8</v>
+      </c>
+      <c r="AE9">
+        <v>62047.753161550849</v>
+      </c>
+      <c r="AF9">
+        <v>0.9738833938764313</v>
+      </c>
+      <c r="AG9">
+        <v>88956.948697178654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P10">
         <v>100</v>
       </c>
       <c r="Q10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD10" s="5">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="AE10">
+        <v>58211.493736215198</v>
+      </c>
+      <c r="AF10">
+        <v>0.97221373888138496</v>
+      </c>
+      <c r="AG10">
+        <v>90152.199242522809</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P11">
         <v>120</v>
       </c>
       <c r="Q11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD11" s="5">
+        <v>148.80000000000001</v>
+      </c>
+      <c r="AE11">
+        <v>32321.777348853899</v>
+      </c>
+      <c r="AF11">
+        <v>0.96316691140479671</v>
+      </c>
+      <c r="AG11">
+        <v>55018.725047026935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P12">
         <v>140</v>
       </c>
       <c r="Q12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD12" s="5">
+        <v>181.2</v>
+      </c>
+      <c r="AE12">
+        <v>12244.765623047355</v>
+      </c>
+      <c r="AF12">
+        <v>0.9758502716844436</v>
+      </c>
+      <c r="AG12">
+        <v>35607.826330715769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P13">
         <v>160</v>
       </c>
       <c r="Q13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD13" s="5">
+        <v>301.2</v>
+      </c>
+      <c r="AE13">
+        <v>7804.7356253636981</v>
+      </c>
+      <c r="AF13">
+        <v>0.96181672025723475</v>
+      </c>
+      <c r="AG13">
+        <v>26784.480310147766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P14">
         <v>180</v>
       </c>
       <c r="Q14">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD14" s="5">
+        <v>619.79999999999995</v>
+      </c>
+      <c r="AE14">
+        <v>5997.7361438029893</v>
+      </c>
+      <c r="AF14">
+        <v>0.92757660167130918</v>
+      </c>
+      <c r="AG14">
+        <v>18091.207088138312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P15">
         <v>240</v>
       </c>
       <c r="Q15">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD15" s="5">
+        <v>915</v>
+      </c>
+      <c r="AE15">
+        <v>5549.3370195194557</v>
+      </c>
+      <c r="AF15">
+        <v>0.87421987518002875</v>
+      </c>
+      <c r="AG15">
+        <v>15843.204817064559</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P16">
         <v>300</v>
       </c>
       <c r="Q16">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD16" s="5">
+        <v>1807.8</v>
+      </c>
+      <c r="AE16">
+        <v>4852.2045218107714</v>
+      </c>
+      <c r="AF16">
+        <v>0.80636042402826857</v>
+      </c>
+      <c r="AG16">
+        <v>12177.168344868838</v>
+      </c>
+    </row>
+    <row r="17" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P17">
         <v>360</v>
       </c>
       <c r="Q17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD17" s="5">
+        <v>2710.2000000000003</v>
+      </c>
+      <c r="AE17">
+        <v>4121.7383597714706</v>
+      </c>
+      <c r="AF17">
+        <v>0.77346278317152117</v>
+      </c>
+      <c r="AG17">
+        <v>9460.2027563540141</v>
+      </c>
+    </row>
+    <row r="18" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P18">
         <v>420</v>
       </c>
       <c r="Q18">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD18" s="5">
+        <v>3610.8</v>
+      </c>
+      <c r="AE18">
+        <v>3449.6509856118491</v>
+      </c>
+      <c r="AF18">
+        <v>0.70903954802259894</v>
+      </c>
+      <c r="AG18">
+        <v>7749.4529025133006</v>
+      </c>
+    </row>
+    <row r="19" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P19">
         <v>480</v>
       </c>
       <c r="Q19">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD19" s="5">
+        <v>4500</v>
+      </c>
+      <c r="AE19">
+        <v>3206.781142108247</v>
+      </c>
+      <c r="AF19">
+        <v>0.68246445497630337</v>
+      </c>
+      <c r="AG19">
+        <v>7079.0657433029664</v>
+      </c>
+    </row>
+    <row r="20" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P20">
         <v>540</v>
       </c>
       <c r="Q20">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD20" s="5">
+        <v>5409</v>
+      </c>
+      <c r="AE20">
+        <v>3442.7536864959579</v>
+      </c>
+      <c r="AF20">
+        <v>0.65989847715736039</v>
+      </c>
+      <c r="AG20">
+        <v>5512.0411957519309</v>
+      </c>
+    </row>
+    <row r="21" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P21">
         <v>660</v>
       </c>
@@ -910,7 +1188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P22">
         <v>780</v>
       </c>
@@ -918,7 +1196,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P23">
         <v>900</v>
       </c>
@@ -926,7 +1204,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P24">
         <v>1020</v>
       </c>
@@ -934,7 +1212,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P25">
         <v>1140</v>
       </c>
@@ -942,7 +1220,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P26">
         <v>1260</v>
       </c>
@@ -950,7 +1228,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P27">
         <v>1380</v>
       </c>
@@ -958,7 +1236,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P28">
         <v>1500</v>
       </c>
@@ -966,7 +1244,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P29">
         <v>1800</v>
       </c>
@@ -974,7 +1252,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P30">
         <v>2100</v>
       </c>
@@ -982,7 +1260,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P31">
         <v>2400</v>
       </c>
@@ -990,7 +1268,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P32">
         <v>2700</v>
       </c>
@@ -998,7 +1276,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P33">
         <v>3000</v>
       </c>
@@ -1006,7 +1284,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P34">
         <v>3300</v>
       </c>
@@ -1014,7 +1292,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P35">
         <v>3600</v>
       </c>
@@ -1022,7 +1300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P36">
         <v>3900</v>
       </c>
@@ -1030,7 +1308,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P37">
         <v>4200</v>
       </c>
@@ -1038,7 +1316,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P38">
         <v>4500</v>
       </c>
@@ -1046,7 +1324,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P39">
         <v>4800</v>
       </c>
@@ -1054,7 +1332,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P40">
         <v>5100</v>
       </c>
@@ -1062,7 +1340,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P41">
         <v>5400</v>
       </c>
@@ -1070,7 +1348,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P42">
         <v>5700</v>
       </c>
@@ -1078,7 +1356,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P43">
         <v>6000</v>
       </c>
@@ -1086,7 +1364,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P44">
         <v>6300</v>
       </c>
@@ -1094,7 +1372,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P45">
         <v>6600</v>
       </c>
@@ -1102,7 +1380,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P46">
         <v>6900</v>
       </c>

</xml_diff>

<commit_message>
Added test for metadata that includes blood data
Updated test in test_dcm2niix4pet to check output of a fully filled
out metadata spreadsheet. Passes the bids-validator and includes
all BIDS columns present in the metadata spreadsheet. Fixed `nii`
entity inclusion for additional blood files by better handling
compressed nii's etc.
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
+++ b/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galassiae/Projects/PET2BIDS/spreadsheet_conversion/single_subject_sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C779BE8-24A2-0444-870D-AC84706497AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CCB3F0-203A-EC4B-B142-DEF8629154B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
215 bug broke metadata extraction w blood data (#217)
* Writes out blood data to bids if provided in xls

Given the required columns in a metadata spreadsheet this writes
out those columns to a _blood.tsv and _blood.json file at the
same location as the output of the imaging files.

Note: The naming of these files is currently incorrect if no subject id
is given nor does it include session or any other entity.

* blood file paths behave the same as nii and sidecar jsons
* bump version, print version via cli
* update metadata injection order
* fixed logging multi prints
* Added test for metadata that includes blood data

Updated test in test_dcm2niix4pet to check output of a fully filled
out metadata spreadsheet. Passes the bids-validator and includes
all BIDS columns present in the metadata spreadsheet. Fixed `nii`
entity inclusion for additional blood files by better handling
compressed nii's etc.
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
+++ b/spreadsheet_conversion/single_subject_sheet/subject_metadata_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\BIDS-converter\Metadata_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galassiae/Projects/PET2BIDS/spreadsheet_conversion/single_subject_sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6621B04B-DC62-40EA-AD7C-D00022C2DFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CCB3F0-203A-EC4B-B142-DEF8629154B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -175,13 +180,25 @@
   </si>
   <si>
     <t>Neurobiology Research Unit</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>plasma_radioactivity</t>
+  </si>
+  <si>
+    <t>metabolite_parent_fraction</t>
+  </si>
+  <si>
+    <t>whole_blood_radioactivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,8 +206,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +224,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -216,11 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +267,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,13 +570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
-  <dimension ref="A1:AC46"/>
+  <dimension ref="A1:AG46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
@@ -569,9 +604,12 @@
     <col min="27" max="27" width="27.83203125" customWidth="1"/>
     <col min="28" max="28" width="15.6640625" customWidth="1"/>
     <col min="29" max="29" width="25.83203125" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,8 +697,20 @@
       <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -748,8 +798,20 @@
       <c r="AC2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD2" s="5">
+        <v>16.200000000000003</v>
+      </c>
+      <c r="AE2">
+        <v>32.35522376080818</v>
+      </c>
+      <c r="AF2">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG2">
+        <v>11.167945849940288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P3">
         <v>10</v>
       </c>
@@ -765,144 +827,360 @@
       <c r="X3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD3" s="5">
+        <v>28.2</v>
+      </c>
+      <c r="AE3">
+        <v>2507.1051839992842</v>
+      </c>
+      <c r="AF3">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG3">
+        <v>4027.7881549527583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P4">
         <v>20</v>
       </c>
       <c r="Q4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD4" s="5">
+        <v>42</v>
+      </c>
+      <c r="AE4">
+        <v>30219.040354280194</v>
+      </c>
+      <c r="AF4">
+        <v>0.9923034124629081</v>
+      </c>
+      <c r="AG4">
+        <v>36565.981242480346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P5">
         <v>30</v>
       </c>
       <c r="Q5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD5" s="5">
+        <v>58.8</v>
+      </c>
+      <c r="AE5">
+        <v>49458.133946955189</v>
+      </c>
+      <c r="AF5">
+        <v>0.987721971939862</v>
+      </c>
+      <c r="AG5">
+        <v>49458.133946955189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P6">
         <v>40</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD6" s="5">
+        <v>73.8</v>
+      </c>
+      <c r="AE6">
+        <v>54625.128373263819</v>
+      </c>
+      <c r="AF6">
+        <v>0.98277401617497218</v>
+      </c>
+      <c r="AG6">
+        <v>77625.006110518632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P7">
         <v>50</v>
       </c>
       <c r="Q7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD7" s="5">
+        <v>88.8</v>
+      </c>
+      <c r="AE7">
+        <v>59463.809533870204</v>
+      </c>
+      <c r="AF7">
+        <v>0.97465638230006379</v>
+      </c>
+      <c r="AG7">
+        <v>84130.176446829675</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P8">
         <v>60</v>
       </c>
       <c r="Q8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD8" s="5">
+        <v>105</v>
+      </c>
+      <c r="AE8">
+        <v>64473.636151116443</v>
+      </c>
+      <c r="AF8">
+        <v>0.97426988808824744</v>
+      </c>
+      <c r="AG8">
+        <v>88701.158697802806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P9">
         <v>80</v>
       </c>
       <c r="Q9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD9" s="5">
+        <v>118.8</v>
+      </c>
+      <c r="AE9">
+        <v>62047.753161550849</v>
+      </c>
+      <c r="AF9">
+        <v>0.9738833938764313</v>
+      </c>
+      <c r="AG9">
+        <v>88956.948697178654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P10">
         <v>100</v>
       </c>
       <c r="Q10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD10" s="5">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="AE10">
+        <v>58211.493736215198</v>
+      </c>
+      <c r="AF10">
+        <v>0.97221373888138496</v>
+      </c>
+      <c r="AG10">
+        <v>90152.199242522809</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P11">
         <v>120</v>
       </c>
       <c r="Q11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD11" s="5">
+        <v>148.80000000000001</v>
+      </c>
+      <c r="AE11">
+        <v>32321.777348853899</v>
+      </c>
+      <c r="AF11">
+        <v>0.96316691140479671</v>
+      </c>
+      <c r="AG11">
+        <v>55018.725047026935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P12">
         <v>140</v>
       </c>
       <c r="Q12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD12" s="5">
+        <v>181.2</v>
+      </c>
+      <c r="AE12">
+        <v>12244.765623047355</v>
+      </c>
+      <c r="AF12">
+        <v>0.9758502716844436</v>
+      </c>
+      <c r="AG12">
+        <v>35607.826330715769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P13">
         <v>160</v>
       </c>
       <c r="Q13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD13" s="5">
+        <v>301.2</v>
+      </c>
+      <c r="AE13">
+        <v>7804.7356253636981</v>
+      </c>
+      <c r="AF13">
+        <v>0.96181672025723475</v>
+      </c>
+      <c r="AG13">
+        <v>26784.480310147766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P14">
         <v>180</v>
       </c>
       <c r="Q14">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD14" s="5">
+        <v>619.79999999999995</v>
+      </c>
+      <c r="AE14">
+        <v>5997.7361438029893</v>
+      </c>
+      <c r="AF14">
+        <v>0.92757660167130918</v>
+      </c>
+      <c r="AG14">
+        <v>18091.207088138312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P15">
         <v>240</v>
       </c>
       <c r="Q15">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD15" s="5">
+        <v>915</v>
+      </c>
+      <c r="AE15">
+        <v>5549.3370195194557</v>
+      </c>
+      <c r="AF15">
+        <v>0.87421987518002875</v>
+      </c>
+      <c r="AG15">
+        <v>15843.204817064559</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="P16">
         <v>300</v>
       </c>
       <c r="Q16">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD16" s="5">
+        <v>1807.8</v>
+      </c>
+      <c r="AE16">
+        <v>4852.2045218107714</v>
+      </c>
+      <c r="AF16">
+        <v>0.80636042402826857</v>
+      </c>
+      <c r="AG16">
+        <v>12177.168344868838</v>
+      </c>
+    </row>
+    <row r="17" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P17">
         <v>360</v>
       </c>
       <c r="Q17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD17" s="5">
+        <v>2710.2000000000003</v>
+      </c>
+      <c r="AE17">
+        <v>4121.7383597714706</v>
+      </c>
+      <c r="AF17">
+        <v>0.77346278317152117</v>
+      </c>
+      <c r="AG17">
+        <v>9460.2027563540141</v>
+      </c>
+    </row>
+    <row r="18" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P18">
         <v>420</v>
       </c>
       <c r="Q18">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD18" s="5">
+        <v>3610.8</v>
+      </c>
+      <c r="AE18">
+        <v>3449.6509856118491</v>
+      </c>
+      <c r="AF18">
+        <v>0.70903954802259894</v>
+      </c>
+      <c r="AG18">
+        <v>7749.4529025133006</v>
+      </c>
+    </row>
+    <row r="19" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P19">
         <v>480</v>
       </c>
       <c r="Q19">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD19" s="5">
+        <v>4500</v>
+      </c>
+      <c r="AE19">
+        <v>3206.781142108247</v>
+      </c>
+      <c r="AF19">
+        <v>0.68246445497630337</v>
+      </c>
+      <c r="AG19">
+        <v>7079.0657433029664</v>
+      </c>
+    </row>
+    <row r="20" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P20">
         <v>540</v>
       </c>
       <c r="Q20">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.35">
+      <c r="AD20" s="5">
+        <v>5409</v>
+      </c>
+      <c r="AE20">
+        <v>3442.7536864959579</v>
+      </c>
+      <c r="AF20">
+        <v>0.65989847715736039</v>
+      </c>
+      <c r="AG20">
+        <v>5512.0411957519309</v>
+      </c>
+    </row>
+    <row r="21" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P21">
         <v>660</v>
       </c>
@@ -910,7 +1188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P22">
         <v>780</v>
       </c>
@@ -918,7 +1196,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P23">
         <v>900</v>
       </c>
@@ -926,7 +1204,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P24">
         <v>1020</v>
       </c>
@@ -934,7 +1212,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P25">
         <v>1140</v>
       </c>
@@ -942,7 +1220,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P26">
         <v>1260</v>
       </c>
@@ -950,7 +1228,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P27">
         <v>1380</v>
       </c>
@@ -958,7 +1236,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P28">
         <v>1500</v>
       </c>
@@ -966,7 +1244,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P29">
         <v>1800</v>
       </c>
@@ -974,7 +1252,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P30">
         <v>2100</v>
       </c>
@@ -982,7 +1260,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P31">
         <v>2400</v>
       </c>
@@ -990,7 +1268,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="16:33" x14ac:dyDescent="0.2">
       <c r="P32">
         <v>2700</v>
       </c>
@@ -998,7 +1276,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P33">
         <v>3000</v>
       </c>
@@ -1006,7 +1284,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P34">
         <v>3300</v>
       </c>
@@ -1014,7 +1292,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P35">
         <v>3600</v>
       </c>
@@ -1022,7 +1300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P36">
         <v>3900</v>
       </c>
@@ -1030,7 +1308,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P37">
         <v>4200</v>
       </c>
@@ -1038,7 +1316,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P38">
         <v>4500</v>
       </c>
@@ -1046,7 +1324,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P39">
         <v>4800</v>
       </c>
@@ -1054,7 +1332,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P40">
         <v>5100</v>
       </c>
@@ -1062,7 +1340,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P41">
         <v>5400</v>
       </c>
@@ -1070,7 +1348,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P42">
         <v>5700</v>
       </c>
@@ -1078,7 +1356,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P43">
         <v>6000</v>
       </c>
@@ -1086,7 +1364,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P44">
         <v>6300</v>
       </c>
@@ -1094,7 +1372,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P45">
         <v>6600</v>
       </c>
@@ -1102,7 +1380,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P46">
         <v>6900</v>
       </c>

</xml_diff>